<commit_message>
remove old spreadsheet files
</commit_message>
<xml_diff>
--- a/test_sheet_colored.xlsx
+++ b/test_sheet_colored.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>Test Table</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Snaaaaaaaaaaaaaaaaaaaaake</t>
+  </si>
+  <si>
+    <t>Non indexed color</t>
   </si>
 </sst>
 </file>
@@ -72,7 +75,7 @@
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,6 +124,12 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -286,7 +295,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -329,6 +338,9 @@
     <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -360,6 +372,7 @@
       <rgbColor rgb="ff88f94e"/>
       <rgbColor rgb="ff72fce9"/>
       <rgbColor rgb="fff27100"/>
+      <rgbColor rgb="ffd397db"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1452,7 +1465,9 @@
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="B5" s="14"/>
+      <c r="B5" t="s" s="14">
+        <v>7</v>
+      </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
@@ -1461,7 +1476,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -1470,7 +1485,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -1479,7 +1494,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="B8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -1488,7 +1503,7 @@
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" s="11"/>
-      <c r="B9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
@@ -1497,7 +1512,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" s="11"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -1506,7 +1521,7 @@
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" s="11"/>
-      <c r="B11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
@@ -1515,7 +1530,7 @@
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" s="11"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1524,7 +1539,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" s="11"/>
-      <c r="B13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -1533,7 +1548,7 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" s="11"/>
-      <c r="B14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -1542,7 +1557,7 @@
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="14"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1551,7 +1566,7 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="14"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1560,7 +1575,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -1569,7 +1584,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -1578,7 +1593,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -1587,7 +1602,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" s="11"/>
-      <c r="B20" s="14"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
@@ -1596,7 +1611,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" s="11"/>
-      <c r="B21" s="14"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -1605,7 +1620,7 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -1614,7 +1629,7 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" s="11"/>
-      <c r="B23" s="14"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>

</xml_diff>